<commit_message>
updated functions to comply with linting and new dependency versions; re-ran plotting notebooks
</commit_message>
<xml_diff>
--- a/experiments/pep_algorithm_benchmarking/exports/result_summary_empkins.xlsx
+++ b/experiments/pep_algorithm_benchmarking/exports/result_summary_empkins.xlsx
@@ -9,9 +9,9 @@
   <sheets>
     <sheet name="pep_describe_total" sheetId="1" r:id="rId1"/>
     <sheet name="hr_describe_total" sheetId="2" r:id="rId2"/>
-    <sheet name="pep_hr_correlation" sheetId="3" r:id="rId3"/>
-    <sheet name="pep_hr_linear_regression" sheetId="4" r:id="rId4"/>
-    <sheet name="describe_pep_phases" sheetId="5" r:id="rId5"/>
+    <sheet name="describe_pep_phases" sheetId="3" r:id="rId3"/>
+    <sheet name="pep_hr_correlation" sheetId="4" r:id="rId4"/>
+    <sheet name="pep_hr_linear_regression" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -38,6 +38,33 @@
     <t>heart_rate_bpm</t>
   </si>
   <si>
+    <t>condition</t>
+  </si>
+  <si>
+    <t>phase</t>
+  </si>
+  <si>
+    <t>TSST</t>
+  </si>
+  <si>
+    <t>f-TSST</t>
+  </si>
+  <si>
+    <t>Preparation</t>
+  </si>
+  <si>
+    <t>Pause 1</t>
+  </si>
+  <si>
+    <t>Talk</t>
+  </si>
+  <si>
+    <t>Math</t>
+  </si>
+  <si>
+    <t>Pause 5</t>
+  </si>
+  <si>
     <t>n</t>
   </si>
   <si>
@@ -93,33 +120,6 @@
   </si>
   <si>
     <t>Intercept</t>
-  </si>
-  <si>
-    <t>condition</t>
-  </si>
-  <si>
-    <t>phase</t>
-  </si>
-  <si>
-    <t>TSST</t>
-  </si>
-  <si>
-    <t>f-TSST</t>
-  </si>
-  <si>
-    <t>Preparation</t>
-  </si>
-  <si>
-    <t>Pause 1</t>
-  </si>
-  <si>
-    <t>Talk</t>
-  </si>
-  <si>
-    <t>Math</t>
-  </si>
-  <si>
-    <t>Pause 5</t>
   </si>
 </sst>
 </file>
@@ -565,168 +565,6 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2">
-        <v>4940</v>
-      </c>
-      <c r="C2">
-        <v>-0.4420842043482303</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2">
-        <v>1.718429509336955E-235</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="B1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2">
-        <v>134.5364851886844</v>
-      </c>
-      <c r="D2">
-        <v>1.370521325583979</v>
-      </c>
-      <c r="E2">
-        <v>98.16445952153163</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0.1954384437342077</v>
-      </c>
-      <c r="H2">
-        <v>0.1952755110577667</v>
-      </c>
-      <c r="I2">
-        <v>131.8496541778291</v>
-      </c>
-      <c r="J2">
-        <v>137.2233161995397</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>-0.4548896055149785</v>
-      </c>
-      <c r="D3">
-        <v>0.01313424493499919</v>
-      </c>
-      <c r="E3">
-        <v>-34.63386039823434</v>
-      </c>
-      <c r="F3">
-        <v>1.718429509317766E-235</v>
-      </c>
-      <c r="G3">
-        <v>0.1954384437342077</v>
-      </c>
-      <c r="H3">
-        <v>0.1952755110577667</v>
-      </c>
-      <c r="I3">
-        <v>-0.4806385639126071</v>
-      </c>
-      <c r="J3">
-        <v>-0.4291406471173499</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -759,18 +597,18 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>81.6896046852123</v>
@@ -788,7 +626,7 @@
     <row r="5" spans="1:6">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>76.61085972850678</v>
@@ -806,7 +644,7 @@
     <row r="6" spans="1:6">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>85.70451612903226</v>
@@ -824,7 +662,7 @@
     <row r="7" spans="1:6">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <v>84.8651832460733</v>
@@ -842,7 +680,7 @@
     <row r="8" spans="1:6">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <v>99.21463414634147</v>
@@ -859,10 +697,10 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <v>87.95417348608838</v>
@@ -880,7 +718,7 @@
     <row r="10" spans="1:6">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="C10">
         <v>78.85388127853881</v>
@@ -898,7 +736,7 @@
     <row r="11" spans="1:6">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="C11">
         <v>93.87951807228916</v>
@@ -916,7 +754,7 @@
     <row r="12" spans="1:6">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="C12">
         <v>94.58832335329342</v>
@@ -934,7 +772,7 @@
     <row r="13" spans="1:6">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="C13">
         <v>111.4947368421053</v>
@@ -957,4 +795,166 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2">
+        <v>4940</v>
+      </c>
+      <c r="C2">
+        <v>-0.4420842043482303</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2">
+        <v>1.718429509336955E-235</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2">
+        <v>134.5364851886843</v>
+      </c>
+      <c r="D2">
+        <v>1.370521325583656</v>
+      </c>
+      <c r="E2">
+        <v>98.16445952155472</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0.1954384437342078</v>
+      </c>
+      <c r="H2">
+        <v>0.1952755110577667</v>
+      </c>
+      <c r="I2">
+        <v>131.8496541778297</v>
+      </c>
+      <c r="J2">
+        <v>137.2233161995389</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>-0.4548896055149778</v>
+      </c>
+      <c r="D3">
+        <v>0.01313424493499633</v>
+      </c>
+      <c r="E3">
+        <v>-34.63386039824183</v>
+      </c>
+      <c r="F3">
+        <v>1.718429508958549E-235</v>
+      </c>
+      <c r="G3">
+        <v>0.1954384437342078</v>
+      </c>
+      <c r="H3">
+        <v>0.1952755110577667</v>
+      </c>
+      <c r="I3">
+        <v>-0.4806385639126008</v>
+      </c>
+      <c r="J3">
+        <v>-0.4291406471173548</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated notebooks and exports (figures, stats)
</commit_message>
<xml_diff>
--- a/experiments/pep_algorithm_benchmarking/exports/result_summary_empkins.xlsx
+++ b/experiments/pep_algorithm_benchmarking/exports/result_summary_empkins.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="57">
   <si>
     <t>mean</t>
   </si>
@@ -83,13 +83,82 @@
     <t>power</t>
   </si>
   <si>
+    <t>ftsst</t>
+  </si>
+  <si>
+    <t>tsst</t>
+  </si>
+  <si>
+    <t>Pause_1</t>
+  </si>
+  <si>
+    <t>Pause_5</t>
+  </si>
+  <si>
+    <t>Prep</t>
+  </si>
+  <si>
     <t>pearson</t>
   </si>
   <si>
-    <t>[-0.46 -0.42]</t>
-  </si>
-  <si>
-    <t>2.143e+231</t>
+    <t>[-0.49 -0.36]</t>
+  </si>
+  <si>
+    <t>[-0.55 -0.34]</t>
+  </si>
+  <si>
+    <t>[-0.41 -0.14]</t>
+  </si>
+  <si>
+    <t>[-0.41 -0.27]</t>
+  </si>
+  <si>
+    <t>[-0.47 -0.35]</t>
+  </si>
+  <si>
+    <t>[-0.46 -0.34]</t>
+  </si>
+  <si>
+    <t>[-0.59 -0.38]</t>
+  </si>
+  <si>
+    <t>[-0.53 -0.31]</t>
+  </si>
+  <si>
+    <t>[-0.58 -0.47]</t>
+  </si>
+  <si>
+    <t>[-0.55 -0.45]</t>
+  </si>
+  <si>
+    <t>3.664e+27</t>
+  </si>
+  <si>
+    <t>1.472e+09</t>
+  </si>
+  <si>
+    <t>159.778</t>
+  </si>
+  <si>
+    <t>5.356e+14</t>
+  </si>
+  <si>
+    <t>1.427e+25</t>
+  </si>
+  <si>
+    <t>1.349e+27</t>
+  </si>
+  <si>
+    <t>6.129e+11</t>
+  </si>
+  <si>
+    <t>2.722e+07</t>
+  </si>
+  <si>
+    <t>2.755e+46</t>
+  </si>
+  <si>
+    <t>1.846e+47</t>
   </si>
   <si>
     <t>names</t>
@@ -799,162 +868,1085 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B2">
-        <v>4940</v>
-      </c>
-      <c r="C2">
-        <v>-0.4420842043482303</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2">
+        <v>662</v>
+      </c>
+      <c r="E2">
+        <v>-0.4277647607103076</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2">
+        <v>7.838484208727989E-31</v>
+      </c>
+      <c r="H2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3">
+        <v>211</v>
+      </c>
+      <c r="E3">
+        <v>-0.4511750823872926</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3">
+        <v>5.621388530288477E-12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3">
+        <v>0.9999997974985221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4">
+        <v>185</v>
+      </c>
+      <c r="E4">
+        <v>-0.2812485256434112</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4">
+        <v>0.0001053020371720138</v>
+      </c>
+      <c r="H4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4">
+        <v>0.9743483049477402</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5">
+        <v>605</v>
+      </c>
+      <c r="E5">
+        <v>-0.3398944541286062</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5">
+        <v>7.945882295800515E-18</v>
+      </c>
+      <c r="H5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5">
+        <v>0.9999999999916147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6">
+        <v>657</v>
+      </c>
+      <c r="E6">
+        <v>-0.4126218282093287</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6">
+        <v>2.133066542065837E-28</v>
+      </c>
+      <c r="H6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E2">
-        <v>1.718429509336955E-235</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7">
+        <v>754</v>
+      </c>
+      <c r="E7">
+        <v>-0.4004840762746094</v>
+      </c>
+      <c r="F7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7">
+        <v>2.050229221963204E-30</v>
+      </c>
+      <c r="H7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G2">
+      <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8">
+        <v>217</v>
+      </c>
+      <c r="E8">
+        <v>-0.4926113309475696</v>
+      </c>
+      <c r="F8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8">
+        <v>1.148363978266648E-14</v>
+      </c>
+      <c r="H8" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8">
+        <v>0.999999998645524</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9">
+        <v>199</v>
+      </c>
+      <c r="E9">
+        <v>-0.4261251552911597</v>
+      </c>
+      <c r="F9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9">
+        <v>3.49382405586447E-10</v>
+      </c>
+      <c r="H9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9">
+        <v>0.9999952123505529</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10">
+        <v>678</v>
+      </c>
+      <c r="E10">
+        <v>-0.5276504258773727</v>
+      </c>
+      <c r="F10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10">
+        <v>7.311302728351472E-50</v>
+      </c>
+      <c r="H10" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10">
         <v>1</v>
       </c>
     </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11">
+        <v>772</v>
+      </c>
+      <c r="E11">
+        <v>-0.5028425796920275</v>
+      </c>
+      <c r="F11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11">
+        <v>1.040711913727697E-50</v>
+      </c>
+      <c r="H11" t="s">
+        <v>46</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:12">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2">
+        <v>143.0230866169004</v>
+      </c>
+      <c r="F2">
+        <v>4.083221433018553</v>
+      </c>
+      <c r="G2">
+        <v>35.02702191469677</v>
+      </c>
+      <c r="H2">
+        <v>1.091631708233266E-152</v>
+      </c>
+      <c r="I2">
+        <v>0.1829826905055467</v>
+      </c>
+      <c r="J2">
+        <v>0.1817447854911611</v>
+      </c>
+      <c r="K2">
+        <v>135.0054166450656</v>
+      </c>
+      <c r="L2">
+        <v>151.0407565887351</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>-0.4904654733182128</v>
+      </c>
+      <c r="F3">
+        <v>0.04034104061853887</v>
+      </c>
+      <c r="G3">
+        <v>-12.15797772685164</v>
+      </c>
+      <c r="H3">
+        <v>7.838484208364906E-31</v>
+      </c>
+      <c r="I3">
+        <v>0.1829826905055467</v>
+      </c>
+      <c r="J3">
+        <v>0.1817447854911611</v>
+      </c>
+      <c r="K3">
+        <v>-0.5696777216142157</v>
+      </c>
+      <c r="L3">
+        <v>-0.41125322502221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4">
+        <v>118.4173171807417</v>
+      </c>
+      <c r="F4">
+        <v>5.553996614575606</v>
+      </c>
+      <c r="G4">
+        <v>21.32109999310653</v>
+      </c>
+      <c r="H4">
+        <v>2.451027397311008E-54</v>
+      </c>
+      <c r="I4">
+        <v>0.2035589549671799</v>
+      </c>
+      <c r="J4">
+        <v>0.1997482322636736</v>
+      </c>
+      <c r="K4">
+        <v>107.468282325273</v>
+      </c>
+      <c r="L4">
+        <v>129.3663520362103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>-0.3883205426052954</v>
+      </c>
+      <c r="F5">
+        <v>0.05313111539222096</v>
+      </c>
+      <c r="G5">
+        <v>-7.308721824088606</v>
+      </c>
+      <c r="H5">
+        <v>5.621388530290531E-12</v>
+      </c>
+      <c r="I5">
+        <v>0.2035589549671799</v>
+      </c>
+      <c r="J5">
+        <v>0.1997482322636736</v>
+      </c>
+      <c r="K5">
+        <v>-0.4930621322585343</v>
+      </c>
+      <c r="L5">
+        <v>-0.2835789529520564</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6">
+        <v>139.1550124925177</v>
+      </c>
+      <c r="F6">
+        <v>7.19980164775514</v>
+      </c>
+      <c r="G6">
+        <v>19.32761752345018</v>
+      </c>
+      <c r="H6">
+        <v>4.52596483296207E-46</v>
+      </c>
+      <c r="I6">
+        <v>0.07910073317659283</v>
+      </c>
+      <c r="J6">
+        <v>0.0740684967458638</v>
+      </c>
+      <c r="K6">
+        <v>124.9497180549049</v>
+      </c>
+      <c r="L6">
+        <v>153.3603069301305</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>-0.3253356009153708</v>
+      </c>
+      <c r="F7">
+        <v>0.08205817506688033</v>
+      </c>
+      <c r="G7">
+        <v>-3.964694567606588</v>
+      </c>
+      <c r="H7">
+        <v>0.0001053020371723162</v>
+      </c>
+      <c r="I7">
+        <v>0.07910073317659283</v>
+      </c>
+      <c r="J7">
+        <v>0.0740684967458638</v>
+      </c>
+      <c r="K7">
+        <v>-0.487237358056369</v>
+      </c>
+      <c r="L7">
+        <v>-0.1634338437743726</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1">
+      <c r="C8" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2">
-        <v>134.5364851886843</v>
-      </c>
-      <c r="D2">
-        <v>1.370521325583656</v>
-      </c>
-      <c r="E2">
-        <v>98.16445952155472</v>
-      </c>
-      <c r="F2">
+      <c r="D8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8">
+        <v>125.1317833697593</v>
+      </c>
+      <c r="F8">
+        <v>4.29443540801778</v>
+      </c>
+      <c r="G8">
+        <v>29.13812212337301</v>
+      </c>
+      <c r="H8">
+        <v>3.611055749170309E-117</v>
+      </c>
+      <c r="I8">
+        <v>0.1155282399473829</v>
+      </c>
+      <c r="J8">
+        <v>0.1140614542756538</v>
+      </c>
+      <c r="K8">
+        <v>116.6979164486981</v>
+      </c>
+      <c r="L8">
+        <v>133.5656502908205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>-0.4158780409269534</v>
+      </c>
+      <c r="F9">
+        <v>0.04686031896995117</v>
+      </c>
+      <c r="G9">
+        <v>-8.874844432741314</v>
+      </c>
+      <c r="H9">
+        <v>7.94588229583392E-18</v>
+      </c>
+      <c r="I9">
+        <v>0.1155282399473829</v>
+      </c>
+      <c r="J9">
+        <v>0.1140614542756538</v>
+      </c>
+      <c r="K9">
+        <v>-0.5079072965849096</v>
+      </c>
+      <c r="L9">
+        <v>-0.3238487852689972</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="1">
         <v>0</v>
       </c>
-      <c r="G2">
-        <v>0.1954384437342078</v>
-      </c>
-      <c r="H2">
-        <v>0.1952755110577667</v>
-      </c>
-      <c r="I2">
-        <v>131.8496541778297</v>
-      </c>
-      <c r="J2">
-        <v>137.2233161995389</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1">
+      <c r="D10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10">
+        <v>134.3229979551467</v>
+      </c>
+      <c r="F10">
+        <v>3.603498286346991</v>
+      </c>
+      <c r="G10">
+        <v>37.27572133559005</v>
+      </c>
+      <c r="H10">
+        <v>4.790563050669945E-164</v>
+      </c>
+      <c r="I10">
+        <v>0.170256773114809</v>
+      </c>
+      <c r="J10">
+        <v>0.1689899895623125</v>
+      </c>
+      <c r="K10">
+        <v>127.2471962484633</v>
+      </c>
+      <c r="L10">
+        <v>141.3987996618302</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D11" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
-        <v>-0.4548896055149778</v>
-      </c>
-      <c r="D3">
-        <v>0.01313424493499633</v>
-      </c>
-      <c r="E3">
-        <v>-34.63386039824183</v>
-      </c>
-      <c r="F3">
-        <v>1.718429508958549E-235</v>
-      </c>
-      <c r="G3">
-        <v>0.1954384437342078</v>
-      </c>
-      <c r="H3">
-        <v>0.1952755110577667</v>
-      </c>
-      <c r="I3">
-        <v>-0.4806385639126008</v>
-      </c>
-      <c r="J3">
-        <v>-0.4291406471173548</v>
+      <c r="E11">
+        <v>-0.4108345263962471</v>
+      </c>
+      <c r="F11">
+        <v>0.03543773395977855</v>
+      </c>
+      <c r="G11">
+        <v>-11.59313761039405</v>
+      </c>
+      <c r="H11">
+        <v>2.133066542063992E-28</v>
+      </c>
+      <c r="I11">
+        <v>0.170256773114809</v>
+      </c>
+      <c r="J11">
+        <v>0.1689899895623125</v>
+      </c>
+      <c r="K11">
+        <v>-0.480419790078387</v>
+      </c>
+      <c r="L11">
+        <v>-0.3412492627141072</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12">
+        <v>123.2148410434557</v>
+      </c>
+      <c r="F12">
+        <v>3.268154008689025</v>
+      </c>
+      <c r="G12">
+        <v>37.70166299258388</v>
+      </c>
+      <c r="H12">
+        <v>1.7694236518563E-175</v>
+      </c>
+      <c r="I12">
+        <v>0.1603874953495269</v>
+      </c>
+      <c r="J12">
+        <v>0.1592709893593002</v>
+      </c>
+      <c r="K12">
+        <v>116.7990507881674</v>
+      </c>
+      <c r="L12">
+        <v>129.6306312987439</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>-0.3493426880590919</v>
+      </c>
+      <c r="F13">
+        <v>0.02914720622220993</v>
+      </c>
+      <c r="G13">
+        <v>-11.9854604724653</v>
+      </c>
+      <c r="H13">
+        <v>2.050229221968416E-30</v>
+      </c>
+      <c r="I13">
+        <v>0.1603874953495269</v>
+      </c>
+      <c r="J13">
+        <v>0.1592709893593002</v>
+      </c>
+      <c r="K13">
+        <v>-0.4065622564001645</v>
+      </c>
+      <c r="L13">
+        <v>-0.2921231197180192</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14">
+        <v>116.5297787598672</v>
+      </c>
+      <c r="F14">
+        <v>4.975762315707051</v>
+      </c>
+      <c r="G14">
+        <v>23.41948255687701</v>
+      </c>
+      <c r="H14">
+        <v>4.396618517077487E-61</v>
+      </c>
+      <c r="I14">
+        <v>0.2426659233779359</v>
+      </c>
+      <c r="J14">
+        <v>0.239143439300624</v>
+      </c>
+      <c r="K14">
+        <v>106.722257057932</v>
+      </c>
+      <c r="L14">
+        <v>126.3373004618025</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>-0.3699658572504274</v>
+      </c>
+      <c r="F15">
+        <v>0.04457401641528648</v>
+      </c>
+      <c r="G15">
+        <v>-8.300034123098431</v>
+      </c>
+      <c r="H15">
+        <v>1.148363978246517E-14</v>
+      </c>
+      <c r="I15">
+        <v>0.2426659233779359</v>
+      </c>
+      <c r="J15">
+        <v>0.239143439300624</v>
+      </c>
+      <c r="K15">
+        <v>-0.4578238789158413</v>
+      </c>
+      <c r="L15">
+        <v>-0.2821078355850135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16">
+        <v>137.6673505417903</v>
+      </c>
+      <c r="F16">
+        <v>6.010320260277564</v>
+      </c>
+      <c r="G16">
+        <v>22.9051605538625</v>
+      </c>
+      <c r="H16">
+        <v>1.91661642512303E-57</v>
+      </c>
+      <c r="I16">
+        <v>0.181582647971915</v>
+      </c>
+      <c r="J16">
+        <v>0.177428245169742</v>
+      </c>
+      <c r="K16">
+        <v>125.8145239702176</v>
+      </c>
+      <c r="L16">
+        <v>149.5201771133629</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>-0.4016605277844157</v>
+      </c>
+      <c r="F17">
+        <v>0.06075419675672439</v>
+      </c>
+      <c r="G17">
+        <v>-6.61123921023545</v>
+      </c>
+      <c r="H17">
+        <v>3.493824055857879E-10</v>
+      </c>
+      <c r="I17">
+        <v>0.181582647971915</v>
+      </c>
+      <c r="J17">
+        <v>0.177428245169742</v>
+      </c>
+      <c r="K17">
+        <v>-0.521472605422255</v>
+      </c>
+      <c r="L17">
+        <v>-0.2818484501465763</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18">
+        <v>134.5628617024328</v>
+      </c>
+      <c r="F18">
+        <v>3.351476706595111</v>
+      </c>
+      <c r="G18">
+        <v>40.15031983890474</v>
+      </c>
+      <c r="H18">
+        <v>3.848917862315853E-181</v>
+      </c>
+      <c r="I18">
+        <v>0.2784149719285728</v>
+      </c>
+      <c r="J18">
+        <v>0.2773475384550943</v>
+      </c>
+      <c r="K18">
+        <v>127.9823060744165</v>
+      </c>
+      <c r="L18">
+        <v>141.1434173304492</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>-0.5316774090998064</v>
+      </c>
+      <c r="F19">
+        <v>0.0329209472905977</v>
+      </c>
+      <c r="G19">
+        <v>-16.15012485535782</v>
+      </c>
+      <c r="H19">
+        <v>7.311302728202795E-50</v>
+      </c>
+      <c r="I19">
+        <v>0.2784149719285728</v>
+      </c>
+      <c r="J19">
+        <v>0.2773475384550943</v>
+      </c>
+      <c r="K19">
+        <v>-0.5963170124562811</v>
+      </c>
+      <c r="L19">
+        <v>-0.4670378057433318</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20">
+        <v>154.5599770143845</v>
+      </c>
+      <c r="F20">
+        <v>4.357781872147626</v>
+      </c>
+      <c r="G20">
+        <v>35.46757996361423</v>
+      </c>
+      <c r="H20">
+        <v>4.404141149836399E-164</v>
+      </c>
+      <c r="I20">
+        <v>0.2528506599513332</v>
+      </c>
+      <c r="J20">
+        <v>0.2518803361330881</v>
+      </c>
+      <c r="K20">
+        <v>146.005434955905</v>
+      </c>
+      <c r="L20">
+        <v>163.114519072864</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21">
+        <v>-0.6106779859996572</v>
+      </c>
+      <c r="F21">
+        <v>0.0378301936905579</v>
+      </c>
+      <c r="G21">
+        <v>-16.1426079653427</v>
+      </c>
+      <c r="H21">
+        <v>1.04071191376313E-50</v>
+      </c>
+      <c r="I21">
+        <v>0.2528506599513332</v>
+      </c>
+      <c r="J21">
+        <v>0.2518803361330881</v>
+      </c>
+      <c r="K21">
+        <v>-0.6849405334379974</v>
+      </c>
+      <c r="L21">
+        <v>-0.5364154385613169</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="A12:A21"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>